<commit_message>
finished and tested chat-box
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuanz\Documents\GitHub\Group04\MediaApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA96B20-63AB-41CC-BFB5-7E4EFC8EB411}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17B820D-C441-4172-BD6B-A3833248792E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{7BC07620-923D-416A-9D18-BE5AD6AD2AE1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>header</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -152,15 +152,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>working</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>customer news feeding service</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chat service</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frontend unit test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frontend function test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backend unit test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backend function test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integration test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Tumula A., Madhu N., Lei J., Yuan Z. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -185,7 +213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,8 +274,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -366,19 +412,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -388,7 +421,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -407,73 +440,79 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -796,255 +835,305 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BFDD44-4111-483F-827E-9D880403D6D8}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16.76171875" customWidth="1"/>
     <col min="2" max="2" width="27.52734375" customWidth="1"/>
-    <col min="3" max="3" width="12.17578125" customWidth="1"/>
+    <col min="3" max="3" width="19.46875" customWidth="1"/>
     <col min="5" max="5" width="21.703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="7"/>
+      <c r="A2" s="13"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="3"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="7"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="7"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="7"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="3"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="7"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="7"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="3"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="7"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="7"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="8"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="28" t="s">
-        <v>30</v>
+      <c r="D11" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="9"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="7"/>
-      <c r="B14" s="4" t="s">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="13"/>
+      <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="7"/>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="13"/>
+      <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="10" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="9"/>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="21"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="18"/>
+      <c r="B18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="7" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C19" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5" t="s">
+      <c r="D19" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="13"/>
+      <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="7"/>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="15"/>
+      <c r="D20" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="13"/>
+      <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
       <c r="C21" s="16"/>
+      <c r="D21" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="16"/>
+      <c r="A22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="13"/>
+      <c r="B24" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="13"/>
+      <c r="B25" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="13"/>
+      <c r="B26" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C1:C7"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="A1:A9"/>
+    <mergeCell ref="A10:A13"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="C1:C7"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="A1:A9"/>
-    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="C24:C26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
all worked except the weather
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuanz\Documents\GitHub\Group04\MediaApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuanz\Documents\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17B820D-C441-4172-BD6B-A3833248792E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA9A020-5258-4D1B-99B5-AAD6A007086A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="18426" windowHeight="11746" xr2:uid="{7BC07620-923D-416A-9D18-BE5AD6AD2AE1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>header</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -189,6 +189,26 @@
   </si>
   <si>
     <t xml:space="preserve">Tumula A., Madhu N., Lei J., Yuan Z. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>route guard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Helper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http interceptor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>news data for db</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anuragreddy Gunreddy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -213,7 +233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,36 +284,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -351,7 +383,9 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -363,6 +397,21 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -371,48 +420,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -421,7 +435,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -434,85 +448,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -835,7 +855,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BFDD44-4111-483F-827E-9D880403D6D8}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
@@ -845,295 +865,357 @@
   <cols>
     <col min="1" max="1" width="16.76171875" customWidth="1"/>
     <col min="2" max="2" width="27.52734375" customWidth="1"/>
-    <col min="3" max="3" width="19.46875" customWidth="1"/>
+    <col min="3" max="3" width="20.46875" customWidth="1"/>
     <col min="5" max="5" width="21.703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="13"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="3"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="13"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="13"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="13"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="13"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="13"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="13"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="13"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="24"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="24"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="18"/>
-      <c r="B13" s="27" t="s">
+      <c r="A13" s="24"/>
+      <c r="B13" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C15" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="13"/>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="17"/>
+      <c r="B16" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="13"/>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="17"/>
+      <c r="B17" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="17" t="s">
+      <c r="C17" s="26"/>
+      <c r="D17" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="18"/>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="26"/>
+      <c r="D18" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="23"/>
+      <c r="B19" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="13" t="s">
+      <c r="C19" s="26"/>
+      <c r="D19" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="24"/>
+      <c r="B20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C21" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="13"/>
-      <c r="B20" s="5" t="s">
+      <c r="D21" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="21"/>
+      <c r="B22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="13"/>
-      <c r="B21" s="5" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="21"/>
+      <c r="B23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="13" t="s">
+      <c r="C23" s="20"/>
+      <c r="D23" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C24" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="13"/>
-      <c r="B23" s="28" t="s">
+      <c r="D24" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="27"/>
+      <c r="B25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="13"/>
-      <c r="B24" s="28" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="27"/>
+      <c r="B26" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C26" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="13"/>
-      <c r="B25" s="28" t="s">
+      <c r="D26" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="27"/>
+      <c r="B27" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="13"/>
-      <c r="B26" s="28" t="s">
+      <c r="C27" s="28"/>
+      <c r="D27" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="27"/>
+      <c r="B28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="3"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A14:A16"/>
+  <mergeCells count="13">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A15:A17"/>
     <mergeCell ref="C1:C7"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="A1:A9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>